<commit_message>
Version 2 - Add fish feeder
</commit_message>
<xml_diff>
--- a/Pecera.xlsx
+++ b/Pecera.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="460" windowWidth="20700" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="9000" yWindow="3460" windowWidth="20700" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Calculos" sheetId="1" r:id="rId1"/>
@@ -441,11 +441,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -714,7 +715,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -756,18 +757,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -780,9 +769,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1065,7 +1067,7 @@
   <dimension ref="B1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1124,21 +1126,21 @@
       </c>
     </row>
     <row r="3" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="45"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="41"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
@@ -1623,19 +1625,19 @@
       <c r="N15" s="27"/>
     </row>
     <row r="16" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="46" t="s">
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="9" t="s">
@@ -1889,42 +1891,42 @@
       </c>
     </row>
     <row r="27" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="39"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="46"/>
+      <c r="N27" s="46"/>
     </row>
     <row r="28" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="41" t="s">
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="46" t="s">
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="K28" s="46"/>
-      <c r="L28" s="46"/>
-      <c r="M28" s="46"/>
-      <c r="N28" s="46"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="42"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="9"/>
@@ -2350,42 +2352,42 @@
       <c r="M41" s="33"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="39" t="s">
+      <c r="B42" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="46"/>
+      <c r="N42" s="46"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="40"/>
-      <c r="F43" s="40" t="s">
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40" t="s">
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="K43" s="40"/>
-      <c r="L43" s="40"/>
-      <c r="M43" s="40"/>
-      <c r="N43" s="40"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="47"/>
+      <c r="M43" s="47"/>
+      <c r="N43" s="47"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B44" s="38"/>
@@ -2749,17 +2751,17 @@
     </sortState>
   </autoFilter>
   <mergeCells count="11">
+    <mergeCell ref="B42:N42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="J43:N43"/>
+    <mergeCell ref="F28:I28"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="E16:J16"/>
     <mergeCell ref="B28:E28"/>
     <mergeCell ref="J28:N28"/>
     <mergeCell ref="B27:N27"/>
-    <mergeCell ref="B42:N42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="J43:N43"/>
-    <mergeCell ref="F28:I28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2768,10 +2770,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:B6"/>
+  <dimension ref="B1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2779,34 +2781,77 @@
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="6">
         <v>42530.875</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="6">
         <v>42531.083333333336</v>
       </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="48">
+        <f>B3-B2</f>
+        <v>0.20833333333575865</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="6">
         <v>42531.25</v>
       </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="48">
+        <f t="shared" ref="C4:C9" si="0">B4-B3</f>
+        <v>0.16666666666424135</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="6">
         <v>42531.583333333336</v>
       </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="48">
+        <f t="shared" si="0"/>
+        <v>0.33333333333575865</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="6">
         <v>42536.611111111109</v>
+      </c>
+      <c r="C6" s="48">
+        <f t="shared" si="0"/>
+        <v>5.0277777777737356</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="6">
+        <v>42571.611111111109</v>
+      </c>
+      <c r="C7" s="48">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="6">
+        <v>42571.791666666664</v>
+      </c>
+      <c r="C8" s="48">
+        <f t="shared" si="0"/>
+        <v>0.18055555555474712</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="6">
+        <v>42572.25</v>
+      </c>
+      <c r="C9" s="48">
+        <f t="shared" si="0"/>
+        <v>0.45833333333575865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>